<commit_message>
chore: rename fields and introduce jsonl
</commit_message>
<xml_diff>
--- a/test_data/datasets/invalid/invalid_format.xlsx
+++ b/test_data/datasets/invalid/invalid_format.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
-    <t>query</t>
+    <t>prompt</t>
   </si>
   <si>
     <t>Wie kann ich mein Passwort zurücksetzen?</t>
@@ -75,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -132,12 +132,74 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -149,7 +211,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -165,10 +227,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1251,14 +1331,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="8.85156" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1267,61 +1347,81 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="A2" t="s" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="A5" t="s" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: default format for datasets now jsonl (#44)
* chore: rename datasets feature to dataset

* chore: rename fields and introduce jsonl

* feat: default format is now jsonl, add tests with bigger files

* chore: fix response type for local upload

* chore: pyright and sonar issues

* fix: log level hardcoding

* chore: fix type

* feat: optimize dataset upload
</commit_message>
<xml_diff>
--- a/test_data/datasets/invalid/invalid_format.xlsx
+++ b/test_data/datasets/invalid/invalid_format.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
-    <t>query</t>
+    <t>prompt</t>
   </si>
   <si>
     <t>Wie kann ich mein Passwort zurücksetzen?</t>
@@ -75,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -132,12 +132,74 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -149,7 +211,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -165,10 +227,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1251,14 +1331,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="8.85156" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1267,61 +1347,81 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="A2" t="s" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="A5" t="s" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>